<commit_message>
update CMMC profile template
</commit_message>
<xml_diff>
--- a/resources/templates/CMMC-2.0-profile-template.xlsx
+++ b/resources/templates/CMMC-2.0-profile-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://opticcybercom.sharepoint.com/sites/Team/Shared Documents/Optic Resources/CMMC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="444" documentId="8_{296C63CC-6ED5-414B-8D6F-633A53BB02DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F2250B0-ED9E-4FE7-BBB4-DEFF198178A5}"/>
+  <xr:revisionPtr revIDLastSave="448" documentId="8_{296C63CC-6ED5-414B-8D6F-633A53BB02DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BDE0589-63DF-4ED2-B00D-D35C337D12F2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{39A0D68A-658D-4156-AFAE-01957333DF12}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{39A0D68A-658D-4156-AFAE-01957333DF12}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="382">
   <si>
     <t>Introduction</t>
   </si>
@@ -562,9 +562,6 @@
     <t>Protect wireless access using authentication and encryption.</t>
   </si>
   <si>
-    <t>Encrypt CUI on mobile devices and mobile computing platforms</t>
-  </si>
-  <si>
     <t>Ensure that managers, systems administrators, and users of organizational systems are made aware of the security risks associated with their activities and of the applicable policies, standards, and procedures related to the security of those systems.</t>
   </si>
   <si>
@@ -607,15 +604,9 @@
     <t>Perform periodic scans of organizational systems and real-time scans of files from external sources as files are downloaded, opened, or executed.</t>
   </si>
   <si>
-    <t>Identify unauthorized use of organizational systems</t>
-  </si>
-  <si>
     <t>Remote Access Confidentiality</t>
   </si>
   <si>
-    <t>Privileged Remote Acces</t>
-  </si>
-  <si>
     <t>Wireless Access Authorization</t>
   </si>
   <si>
@@ -700,9 +691,6 @@
     <t>AT.L2-3.2.3</t>
   </si>
   <si>
-    <t>Audit and Accountabiltiy</t>
-  </si>
-  <si>
     <t>System Auditing</t>
   </si>
   <si>
@@ -1000,9 +988,6 @@
     <t>Monitor Facility</t>
   </si>
   <si>
-    <t>Alternateive Work Site</t>
-  </si>
-  <si>
     <t>PE.L2-3.10.2</t>
   </si>
   <si>
@@ -1012,12 +997,6 @@
     <t>Risk Assessments</t>
   </si>
   <si>
-    <t>Vulnerabilty Scan</t>
-  </si>
-  <si>
-    <t>Vulnerabilty Remediation</t>
-  </si>
-  <si>
     <t>Security Assessments</t>
   </si>
   <si>
@@ -1148,9 +1127,6 @@
   </si>
   <si>
     <t>Flaw Remediation</t>
-  </si>
-  <si>
-    <t>Maliciuos Code Protection</t>
   </si>
   <si>
     <t>Update Malicious Code Protection</t>
@@ -1200,7 +1176,28 @@
 </t>
   </si>
   <si>
-    <t>This CMMC Profile is a job aid to help organization prepare for CMMC Certification.  This aid is not a definitive source of requirements or expectations of the DoD. However, it does provide the CMMC controls as released by Office of the Under Secretary of Defense for Acquisition &amp; Sustainment.  While this profile may not represent all the information required in a System Security Plan (SSP) as required by CMMC, it is a starter guide to help get started in defining capabiliteis currently in place to assist in identifying gaps that should be corrected prior to developing a formal SSP.</t>
+    <t>Privileged Remote Access</t>
+  </si>
+  <si>
+    <t>Alternative Work Site</t>
+  </si>
+  <si>
+    <t>Vulnerability Scan</t>
+  </si>
+  <si>
+    <t>Vulnerability Remediation</t>
+  </si>
+  <si>
+    <t>Malicious Code Protection</t>
+  </si>
+  <si>
+    <t>Identify unauthorized use of organizational systems.</t>
+  </si>
+  <si>
+    <t>Encrypt CUI on mobile devices and mobile computing platforms.</t>
+  </si>
+  <si>
+    <t>This CMMC Profile is a job aid to help organization prepare for CMMC Certification.  This aid is not a definitive source of requirements or expectations of the DoD. However, it does provide the CMMC controls as released by Office of the Under Secretary of Defense for Acquisition &amp; Sustainment.  While this profile may not represent all the information required in a System Security Plan (SSP) as required by CMMC, it is a starter guide to help get started in defining capabilities currently in place to assist in identifying gaps that should be corrected prior to developing a formal SSP.</t>
   </si>
 </sst>
 </file>
@@ -1948,19 +1945,19 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AT22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:L7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.23046875" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
     <col min="3" max="46" width="9" style="1"/>
-    <col min="47" max="16384" width="9.26953125" style="2"/>
+    <col min="47" max="16384" width="9.23046875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="66.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="66.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22"/>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1974,7 +1971,7 @@
       <c r="K1" s="23"/>
       <c r="L1" s="24"/>
     </row>
-    <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
@@ -1989,9 +1986,9 @@
       <c r="K3" s="26"/>
       <c r="L3" s="27"/>
     </row>
-    <row r="4" spans="1:12" ht="43" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="43" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="21" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
@@ -2004,7 +2001,7 @@
       <c r="K4" s="21"/>
       <c r="L4" s="21"/>
     </row>
-    <row r="5" spans="1:12" ht="38.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
@@ -2017,7 +2014,7 @@
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
     </row>
-    <row r="6" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
@@ -2030,7 +2027,7 @@
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
@@ -2043,8 +2040,8 @@
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
     </row>
-    <row r="8" spans="1:12" ht="7.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:12" ht="20" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="7.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:12" ht="20.149999999999999" x14ac:dyDescent="0.5">
       <c r="B9" s="25" t="s">
         <v>1</v>
       </c>
@@ -2059,9 +2056,9 @@
       <c r="K9" s="26"/>
       <c r="L9" s="27"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B10" s="21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
@@ -2074,7 +2071,7 @@
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -2087,7 +2084,7 @@
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -2100,7 +2097,7 @@
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -2113,8 +2110,8 @@
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:12" ht="20" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="23.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:12" ht="20.149999999999999" x14ac:dyDescent="0.5">
       <c r="B15" s="25" t="s">
         <v>2</v>
       </c>
@@ -2129,9 +2126,9 @@
       <c r="K15" s="26"/>
       <c r="L15" s="27"/>
     </row>
-    <row r="16" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="21" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -2144,7 +2141,7 @@
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
     </row>
-    <row r="17" spans="2:12" ht="40.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="40.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -2157,7 +2154,7 @@
       <c r="K17" s="21"/>
       <c r="L17" s="21"/>
     </row>
-    <row r="18" spans="2:12" ht="29.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
@@ -2170,12 +2167,12 @@
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>4</v>
       </c>
@@ -2205,12 +2202,12 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" customWidth="1"/>
+    <col min="1" max="1" width="37.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2218,7 +2215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -2226,7 +2223,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2234,7 +2231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2242,7 +2239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2250,7 +2247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2258,7 +2255,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2266,7 +2263,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2274,7 +2271,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2282,7 +2279,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2290,7 +2287,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2298,7 +2295,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -2306,7 +2303,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -2314,7 +2311,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2322,7 +2319,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -2330,7 +2327,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2338,7 +2335,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2356,25 +2353,25 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:EO112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L67" sqref="L67"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" style="4"/>
-    <col min="3" max="3" width="16.81640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="33.6328125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="67.54296875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="60.26953125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="54.81640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="15.4609375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="9.15234375" style="4"/>
+    <col min="3" max="3" width="16.84375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="33.61328125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="67.53515625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="60.23046875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="54.84375" style="10" customWidth="1"/>
     <col min="8" max="8" width="13" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="4"/>
+    <col min="9" max="16384" width="9.15234375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="28"/>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -2383,7 +2380,7 @@
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
     </row>
-    <row r="2" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>42</v>
       </c>
@@ -2406,10 +2403,10 @@
         <v>47</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -2432,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -2456,7 +2453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -2480,7 +2477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -2504,7 +2501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2528,7 +2525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -2537,7 +2534,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>163</v>
@@ -2552,7 +2549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -2561,7 +2558,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>138</v>
@@ -2576,7 +2573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -2585,7 +2582,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>164</v>
@@ -2600,7 +2597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -2609,7 +2606,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>165</v>
@@ -2624,7 +2621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -2633,7 +2630,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>166</v>
@@ -2648,7 +2645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -2657,7 +2654,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>167</v>
@@ -2672,7 +2669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -2681,7 +2678,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>168</v>
@@ -2696,7 +2693,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2705,7 +2702,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>139</v>
@@ -2720,7 +2717,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
@@ -2729,7 +2726,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>140</v>
@@ -2744,7 +2741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
@@ -2753,10 +2750,10 @@
         <v>2</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>61</v>
@@ -2768,7 +2765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
@@ -2777,7 +2774,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>141</v>
@@ -2792,7 +2789,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
@@ -2801,10 +2798,10 @@
         <v>2</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>187</v>
+        <v>374</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>66</v>
@@ -2816,7 +2813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
@@ -2825,10 +2822,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>58</v>
@@ -2840,7 +2837,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>5</v>
       </c>
@@ -2849,10 +2846,10 @@
         <v>2</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>169</v>
@@ -2864,7 +2861,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
@@ -2873,10 +2870,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>65</v>
@@ -2888,7 +2885,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2897,13 +2894,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>170</v>
+        <v>380</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
@@ -2912,7 +2909,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -2921,10 +2918,10 @@
         <v>2</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>53</v>
@@ -2936,7 +2933,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="56.6" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>6</v>
       </c>
@@ -2945,13 +2942,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
@@ -2960,7 +2957,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
@@ -2969,13 +2966,13 @@
         <v>2</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
@@ -2984,7 +2981,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>6</v>
       </c>
@@ -2993,10 +2990,10 @@
         <v>2</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>77</v>
@@ -3008,19 +3005,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>216</v>
+        <v>7</v>
       </c>
       <c r="B28" s="12" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>69</v>
@@ -3032,19 +3029,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>216</v>
+        <v>7</v>
       </c>
       <c r="B29" s="12" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>68</v>
@@ -3056,19 +3053,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>216</v>
+        <v>7</v>
       </c>
       <c r="B30" s="12" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>71</v>
@@ -3080,16 +3077,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>216</v>
+        <v>7</v>
       </c>
       <c r="B31" s="12" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>142</v>
@@ -3104,16 +3101,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>216</v>
+        <v>7</v>
       </c>
       <c r="B32" s="12" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>143</v>
@@ -3128,19 +3125,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:145" s="13" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:145" s="13" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>216</v>
+        <v>7</v>
       </c>
       <c r="B33" s="12" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>76</v>
@@ -3289,19 +3286,19 @@
       <c r="EN33" s="4"/>
       <c r="EO33" s="4"/>
     </row>
-    <row r="34" spans="1:145" s="14" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:145" s="14" customFormat="1" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>216</v>
+        <v>7</v>
       </c>
       <c r="B34" s="12" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>70</v>
@@ -3450,19 +3447,19 @@
       <c r="EN34" s="4"/>
       <c r="EO34" s="4"/>
     </row>
-    <row r="35" spans="1:145" s="14" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:145" s="14" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>216</v>
+        <v>7</v>
       </c>
       <c r="B35" s="12" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>73</v>
@@ -3611,19 +3608,19 @@
       <c r="EN35" s="4"/>
       <c r="EO35" s="4"/>
     </row>
-    <row r="36" spans="1:145" s="15" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:145" s="15" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>216</v>
+        <v>7</v>
       </c>
       <c r="B36" s="12" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>74</v>
@@ -3772,7 +3769,7 @@
       <c r="EN36" s="4"/>
       <c r="EO36" s="4"/>
     </row>
-    <row r="37" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>8</v>
       </c>
@@ -3781,10 +3778,10 @@
         <v>2</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>78</v>
@@ -3796,7 +3793,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:145" s="16" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:145" s="16" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>8</v>
       </c>
@@ -3805,10 +3802,10 @@
         <v>2</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>81</v>
@@ -3957,7 +3954,7 @@
       <c r="EN38" s="4"/>
       <c r="EO38" s="4"/>
     </row>
-    <row r="39" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>8</v>
       </c>
@@ -3966,13 +3963,13 @@
         <v>2</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
@@ -3981,7 +3978,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>8</v>
       </c>
@@ -3990,10 +3987,10 @@
         <v>2</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>82</v>
@@ -4005,7 +4002,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>8</v>
       </c>
@@ -4014,10 +4011,10 @@
         <v>2</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>83</v>
@@ -4029,7 +4026,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>8</v>
       </c>
@@ -4038,7 +4035,7 @@
         <v>2</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>144</v>
@@ -4053,7 +4050,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>8</v>
       </c>
@@ -4062,10 +4059,10 @@
         <v>2</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>84</v>
@@ -4077,7 +4074,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>8</v>
       </c>
@@ -4086,13 +4083,13 @@
         <v>2</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
@@ -4101,7 +4098,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>8</v>
       </c>
@@ -4110,10 +4107,10 @@
         <v>2</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>80</v>
@@ -4125,7 +4122,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>9</v>
       </c>
@@ -4134,13 +4131,13 @@
         <v>1</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
@@ -4149,7 +4146,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>9</v>
       </c>
@@ -4158,13 +4155,13 @@
         <v>1</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
@@ -4173,7 +4170,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>9</v>
       </c>
@@ -4182,13 +4179,13 @@
         <v>2</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
@@ -4197,7 +4194,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>9</v>
       </c>
@@ -4206,13 +4203,13 @@
         <v>2</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
@@ -4221,7 +4218,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:145" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:145" s="13" customFormat="1" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>9</v>
       </c>
@@ -4230,13 +4227,13 @@
         <v>2</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
@@ -4382,7 +4379,7 @@
       <c r="EN50" s="4"/>
       <c r="EO50" s="4"/>
     </row>
-    <row r="51" spans="1:145" s="14" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:145" s="14" customFormat="1" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>9</v>
       </c>
@@ -4391,10 +4388,10 @@
         <v>2</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>89</v>
@@ -4543,7 +4540,7 @@
       <c r="EN51" s="4"/>
       <c r="EO51" s="4"/>
     </row>
-    <row r="52" spans="1:145" s="15" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:145" s="15" customFormat="1" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>9</v>
       </c>
@@ -4552,10 +4549,10 @@
         <v>2</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>85</v>
@@ -4704,7 +4701,7 @@
       <c r="EN52" s="4"/>
       <c r="EO52" s="4"/>
     </row>
-    <row r="53" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>9</v>
       </c>
@@ -4713,10 +4710,10 @@
         <v>2</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>86</v>
@@ -4728,7 +4725,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>9</v>
       </c>
@@ -4737,10 +4734,10 @@
         <v>2</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>87</v>
@@ -4752,7 +4749,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>9</v>
       </c>
@@ -4761,13 +4758,13 @@
         <v>2</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
@@ -4776,7 +4773,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:145" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:145" s="13" customFormat="1" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>9</v>
       </c>
@@ -4785,10 +4782,10 @@
         <v>2</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>88</v>
@@ -4937,7 +4934,7 @@
       <c r="EN56" s="4"/>
       <c r="EO56" s="4"/>
     </row>
-    <row r="57" spans="1:145" s="15" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:145" s="15" customFormat="1" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>10</v>
       </c>
@@ -4946,10 +4943,10 @@
         <v>2</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>90</v>
@@ -5098,7 +5095,7 @@
       <c r="EN57" s="4"/>
       <c r="EO57" s="4"/>
     </row>
-    <row r="58" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>10</v>
       </c>
@@ -5107,7 +5104,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D58" s="14" t="s">
         <v>145</v>
@@ -5122,7 +5119,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>10</v>
       </c>
@@ -5131,7 +5128,7 @@
         <v>2</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D59" s="14" t="s">
         <v>146</v>
@@ -5146,7 +5143,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:145" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:145" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>11</v>
       </c>
@@ -5155,10 +5152,10 @@
         <v>2</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>93</v>
@@ -5170,7 +5167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>11</v>
       </c>
@@ -5179,10 +5176,10 @@
         <v>2</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>94</v>
@@ -5194,7 +5191,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>11</v>
       </c>
@@ -5203,13 +5200,13 @@
         <v>2</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
@@ -5218,7 +5215,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>11</v>
       </c>
@@ -5227,10 +5224,10 @@
         <v>2</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>96</v>
@@ -5242,7 +5239,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>11</v>
       </c>
@@ -5251,10 +5248,10 @@
         <v>2</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>95</v>
@@ -5266,7 +5263,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>11</v>
       </c>
@@ -5275,13 +5272,13 @@
         <v>2</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
@@ -5290,7 +5287,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>12</v>
       </c>
@@ -5299,13 +5296,13 @@
         <v>1</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
@@ -5314,7 +5311,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:145" s="13" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:145" s="13" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>12</v>
       </c>
@@ -5323,7 +5320,7 @@
         <v>2</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D67" s="14" t="s">
         <v>12</v>
@@ -5475,7 +5472,7 @@
       <c r="EN67" s="4"/>
       <c r="EO67" s="4"/>
     </row>
-    <row r="68" spans="1:145" s="15" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:145" s="15" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>12</v>
       </c>
@@ -5484,10 +5481,10 @@
         <v>2</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>98</v>
@@ -5636,7 +5633,7 @@
       <c r="EN68" s="4"/>
       <c r="EO68" s="4"/>
     </row>
-    <row r="69" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>12</v>
       </c>
@@ -5645,7 +5642,7 @@
         <v>2</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D69" s="14" t="s">
         <v>147</v>
@@ -5660,7 +5657,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>12</v>
       </c>
@@ -5669,7 +5666,7 @@
         <v>2</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D70" s="14" t="s">
         <v>148</v>
@@ -5684,7 +5681,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>12</v>
       </c>
@@ -5693,10 +5690,10 @@
         <v>2</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>103</v>
@@ -5708,7 +5705,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>12</v>
       </c>
@@ -5717,10 +5714,10 @@
         <v>2</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>99</v>
@@ -5732,7 +5729,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>12</v>
       </c>
@@ -5741,10 +5738,10 @@
         <v>2</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>101</v>
@@ -5756,7 +5753,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>12</v>
       </c>
@@ -5765,10 +5762,10 @@
         <v>2</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>111</v>
@@ -5780,7 +5777,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>13</v>
       </c>
@@ -5789,10 +5786,10 @@
         <v>2</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>104</v>
@@ -5804,7 +5801,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>13</v>
       </c>
@@ -5813,10 +5810,10 @@
         <v>2</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>105</v>
@@ -5828,7 +5825,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>14</v>
       </c>
@@ -5837,13 +5834,13 @@
         <v>1</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D77" s="14" t="s">
         <v>149</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
@@ -5852,7 +5849,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>14</v>
       </c>
@@ -5861,7 +5858,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D78" s="14" t="s">
         <v>150</v>
@@ -5876,7 +5873,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>14</v>
       </c>
@@ -5885,10 +5882,10 @@
         <v>1</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>107</v>
@@ -5900,7 +5897,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>14</v>
       </c>
@@ -5909,10 +5906,10 @@
         <v>1</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>108</v>
@@ -5924,7 +5921,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>14</v>
       </c>
@@ -5933,10 +5930,10 @@
         <v>2</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>109</v>
@@ -5948,7 +5945,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:145" ht="28" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:145" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>14</v>
       </c>
@@ -5957,10 +5954,10 @@
         <v>2</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>316</v>
+        <v>375</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>110</v>
@@ -5972,7 +5969,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:145" ht="56" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:145" ht="56.6" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>15</v>
       </c>
@@ -5981,10 +5978,10 @@
         <v>2</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>112</v>
@@ -5996,7 +5993,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:145" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:145" s="13" customFormat="1" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>15</v>
       </c>
@@ -6005,10 +6002,10 @@
         <v>2</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>320</v>
+        <v>376</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>113</v>
@@ -6157,7 +6154,7 @@
       <c r="EN84" s="4"/>
       <c r="EO84" s="4"/>
     </row>
-    <row r="85" spans="1:145" s="14" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:145" s="14" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>15</v>
       </c>
@@ -6166,10 +6163,10 @@
         <v>2</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>321</v>
+        <v>377</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>114</v>
@@ -6318,16 +6315,16 @@
       <c r="EN85" s="4"/>
       <c r="EO85" s="4"/>
     </row>
-    <row r="86" spans="1:145" s="14" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:145" s="14" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B86" s="12" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D86" s="14" t="s">
         <v>151</v>
@@ -6479,19 +6476,19 @@
       <c r="EN86" s="4"/>
       <c r="EO86" s="4"/>
     </row>
-    <row r="87" spans="1:145" s="14" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:145" s="14" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B87" s="12" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>117</v>
@@ -6640,19 +6637,19 @@
       <c r="EN87" s="4"/>
       <c r="EO87" s="4"/>
     </row>
-    <row r="88" spans="1:145" s="14" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:145" s="14" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B88" s="12" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>118</v>
@@ -6801,19 +6798,19 @@
       <c r="EN88" s="4"/>
       <c r="EO88" s="4"/>
     </row>
-    <row r="89" spans="1:145" s="15" customFormat="1" ht="56" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:145" s="15" customFormat="1" ht="56.6" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B89" s="12" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>115</v>
@@ -6962,7 +6959,7 @@
       <c r="EN89" s="4"/>
       <c r="EO89" s="4"/>
     </row>
-    <row r="90" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>17</v>
       </c>
@@ -6971,13 +6968,13 @@
         <v>1</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
@@ -6986,7 +6983,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>17</v>
       </c>
@@ -6995,10 +6992,10 @@
         <v>1</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>119</v>
@@ -7010,7 +7007,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>17</v>
       </c>
@@ -7019,10 +7016,10 @@
         <v>2</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>122</v>
@@ -7034,7 +7031,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
         <v>17</v>
       </c>
@@ -7043,10 +7040,10 @@
         <v>2</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>123</v>
@@ -7058,7 +7055,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
         <v>17</v>
       </c>
@@ -7067,10 +7064,10 @@
         <v>2</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>124</v>
@@ -7082,7 +7079,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
         <v>17</v>
       </c>
@@ -7091,10 +7088,10 @@
         <v>2</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="E95" s="6" t="s">
         <v>125</v>
@@ -7106,7 +7103,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>17</v>
       </c>
@@ -7115,10 +7112,10 @@
         <v>2</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="E96" s="6" t="s">
         <v>126</v>
@@ -7130,7 +7127,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>17</v>
       </c>
@@ -7139,10 +7136,10 @@
         <v>2</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>127</v>
@@ -7154,7 +7151,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
         <v>17</v>
       </c>
@@ -7163,10 +7160,10 @@
         <v>2</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>128</v>
@@ -7178,7 +7175,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>17</v>
       </c>
@@ -7187,10 +7184,10 @@
         <v>2</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>129</v>
@@ -7202,7 +7199,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>17</v>
       </c>
@@ -7211,10 +7208,10 @@
         <v>2</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>121</v>
@@ -7226,7 +7223,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
         <v>17</v>
       </c>
@@ -7235,10 +7232,10 @@
         <v>2</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>120</v>
@@ -7250,7 +7247,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>17</v>
       </c>
@@ -7259,10 +7256,10 @@
         <v>2</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>130</v>
@@ -7274,7 +7271,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>17</v>
       </c>
@@ -7283,10 +7280,10 @@
         <v>2</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>152</v>
@@ -7298,7 +7295,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
         <v>17</v>
       </c>
@@ -7307,10 +7304,10 @@
         <v>2</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>131</v>
@@ -7322,7 +7319,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
         <v>17</v>
       </c>
@@ -7331,10 +7328,10 @@
         <v>2</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="E105" s="6" t="s">
         <v>18</v>
@@ -7346,7 +7343,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>19</v>
       </c>
@@ -7355,10 +7352,10 @@
         <v>1</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>132</v>
@@ -7370,7 +7367,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
         <v>19</v>
       </c>
@@ -7379,10 +7376,10 @@
         <v>1</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>366</v>
+        <v>378</v>
       </c>
       <c r="E107" s="6" t="s">
         <v>133</v>
@@ -7394,7 +7391,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>19</v>
       </c>
@@ -7403,10 +7400,10 @@
         <v>1</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>134</v>
@@ -7418,7 +7415,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
         <v>19</v>
       </c>
@@ -7427,13 +7424,13 @@
         <v>1</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
@@ -7442,7 +7439,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>19</v>
       </c>
@@ -7451,10 +7448,10 @@
         <v>2</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="D110" s="14" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>135</v>
@@ -7466,7 +7463,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:145" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:145" s="16" customFormat="1" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
         <v>19</v>
       </c>
@@ -7475,10 +7472,10 @@
         <v>2</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>136</v>
@@ -7627,7 +7624,7 @@
       <c r="EN111" s="4"/>
       <c r="EO111" s="4"/>
     </row>
-    <row r="112" spans="1:145" ht="42" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>19</v>
       </c>
@@ -7636,13 +7633,13 @@
         <v>2</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>185</v>
+        <v>379</v>
       </c>
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
@@ -7884,6 +7881,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="a54a5347-8adb-4f47-b158-08c1baf179b6">
@@ -7900,15 +7906,6 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7931,6 +7928,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27AF1D4A-D486-4D3A-B452-4FB4D8FA194C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A3B4A12-2BF8-4469-B875-58751C987CB1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7939,12 +7944,4 @@
     <ds:schemaRef ds:uri="9e79c3b1-452c-4fb6-ac46-d68c59ca6476"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27AF1D4A-D486-4D3A-B452-4FB4D8FA194C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update CMMC 2.0 Profile template
</commit_message>
<xml_diff>
--- a/resources/templates/CMMC-2.0-profile-template.xlsx
+++ b/resources/templates/CMMC-2.0-profile-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://opticcybercom.sharepoint.com/sites/Team/Shared Documents/Optic Resources/CMMC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://opticcybercom.sharepoint.com/sites/marketing/Shared Documents/Website/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="448" documentId="8_{296C63CC-6ED5-414B-8D6F-633A53BB02DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BDE0589-63DF-4ED2-B00D-D35C337D12F2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8271387C-5F03-470A-BBC7-4AD838C2E867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{39A0D68A-658D-4156-AFAE-01957333DF12}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{39A0D68A-658D-4156-AFAE-01957333DF12}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="4" r:id="rId1"/>
@@ -253,9 +253,6 @@
     <t>Authorize remote execution of privileged commands and remote access to security-relevant information.</t>
   </si>
   <si>
-    <t>Control information flows between security domains on connected systems.</t>
-  </si>
-  <si>
     <t>Ensure that the actions of individual system users can be uniquely traced to those users so they can be held accountable for their actions.</t>
   </si>
   <si>
@@ -565,18 +562,12 @@
     <t>Ensure that managers, systems administrators, and users of organizational systems are made aware of the security risks associated with their activities and of the applicable policies, standards, and procedures related to the security of those systems.</t>
   </si>
   <si>
-    <t>Ensure that personnel are trained to carry out their assigned information security related duties and responsibilities.</t>
-  </si>
-  <si>
     <t>Track, review, approve or disapprove, and log changes to organizational systems.</t>
   </si>
   <si>
     <t>Apply deny-by-exception (blacklisting) policy to prevent the use of unauthorized software or deny-all, permit-by-exception (whitelisting) policy to allow the execution of authorized software.</t>
   </si>
   <si>
-    <t>Use multifactor authentication (MFA) for local and network access to privileged accounts and for network access to nonprivileged accounts.</t>
-  </si>
-  <si>
     <t>Employ replay-resistant authentication mechanisms for network access to privileged and non-privileged accounts.</t>
   </si>
   <si>
@@ -590,15 +581,6 @@
   </si>
   <si>
     <t>Supervise the maintenance activities of maintenance personnel without required access authorization.</t>
-  </si>
-  <si>
-    <t>Sanitize or destroy system media containing CUI before disposal or release for reuse.</t>
-  </si>
-  <si>
-    <t>Limit physical access to organizational systems, equipment, and the respective operating environments to authorized individuals.</t>
-  </si>
-  <si>
-    <t>Monitor, control, and protect communications (i.e., information transmitted or received by organizational systems) at the external boundaries and key internal boundaries of organizational systems.</t>
   </si>
   <si>
     <t>Perform periodic scans of organizational systems and real-time scans of files from external sources as files are downloaded, opened, or executed.</t>
@@ -1198,6 +1180,24 @@
   </si>
   <si>
     <t>This CMMC Profile is a job aid to help organization prepare for CMMC Certification.  This aid is not a definitive source of requirements or expectations of the DoD. However, it does provide the CMMC controls as released by Office of the Under Secretary of Defense for Acquisition &amp; Sustainment.  While this profile may not represent all the information required in a System Security Plan (SSP) as required by CMMC, it is a starter guide to help get started in defining capabilities currently in place to assist in identifying gaps that should be corrected prior to developing a formal SSP.</t>
+  </si>
+  <si>
+    <t>Control the flow of CUI in accordance with approved authorizations.</t>
+  </si>
+  <si>
+    <t>Ensure that personnel are trained to carry out their assigned information security-related duties and responsibilities.</t>
+  </si>
+  <si>
+    <t>Use multifactor authentication for local and network access to privileged accounts and for network access to nonprivileged accounts.</t>
+  </si>
+  <si>
+    <t>Sanitize or destroy information system media containing Federal Contract Information before disposal or release for reuse.</t>
+  </si>
+  <si>
+    <t>Limit physical access to organizational information systems, equipment, and the respective operating environments to authorized individuals.</t>
+  </si>
+  <si>
+    <t>Monitor, control, and protect organizational communications (i.e., information transmitted or received by organizational information systems) at the external boundaries and key internal boundaries of the information systems.</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1254,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="204"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1601,9 +1601,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>257285</xdr:colOff>
+      <xdr:colOff>263636</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>642463</xdr:rowOff>
+      <xdr:rowOff>644580</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1945,7 +1945,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AT22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10:L13"/>
     </sheetView>
   </sheetViews>
@@ -1957,7 +1957,7 @@
     <col min="47" max="16384" width="9.23046875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="66.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="66.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22"/>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="4" spans="1:12" ht="43" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="21" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
@@ -2001,7 +2001,7 @@
       <c r="K4" s="21"/>
       <c r="L4" s="21"/>
     </row>
-    <row r="5" spans="1:12" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="38.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B10" s="21" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
@@ -2128,7 +2128,7 @@
     </row>
     <row r="16" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="21" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -2353,7 +2353,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:EO112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
@@ -2391,7 +2391,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>45</v>
@@ -2403,7 +2403,7 @@
         <v>47</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="42.45" x14ac:dyDescent="0.35">
@@ -2415,10 +2415,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>154</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>48</v>
@@ -2438,10 +2438,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>155</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>156</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>49</v>
@@ -2462,10 +2462,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>50</v>
@@ -2486,10 +2486,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>159</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>160</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>51</v>
@@ -2501,7 +2501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2510,13 +2510,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>162</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>67</v>
+        <v>376</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
@@ -2534,10 +2534,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>62</v>
@@ -2558,10 +2558,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>54</v>
@@ -2582,10 +2582,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>55</v>
@@ -2606,10 +2606,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>63</v>
@@ -2630,10 +2630,10 @@
         <v>2</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>56</v>
@@ -2654,10 +2654,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>52</v>
@@ -2678,10 +2678,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>57</v>
@@ -2702,10 +2702,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>64</v>
@@ -2726,10 +2726,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>59</v>
@@ -2750,10 +2750,10 @@
         <v>2</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>61</v>
@@ -2774,10 +2774,10 @@
         <v>2</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>60</v>
@@ -2798,10 +2798,10 @@
         <v>2</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>66</v>
@@ -2822,10 +2822,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>58</v>
@@ -2846,13 +2846,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
@@ -2870,10 +2870,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>65</v>
@@ -2894,13 +2894,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
@@ -2918,10 +2918,10 @@
         <v>2</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>53</v>
@@ -2942,13 +2942,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
@@ -2966,13 +2966,13 @@
         <v>2</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>171</v>
+        <v>377</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
@@ -2990,13 +2990,13 @@
         <v>2</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
@@ -3014,13 +3014,13 @@
         <v>2</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
@@ -3038,13 +3038,13 @@
         <v>2</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
@@ -3062,13 +3062,13 @@
         <v>2</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
@@ -3086,13 +3086,13 @@
         <v>2</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
@@ -3110,13 +3110,13 @@
         <v>2</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
@@ -3134,13 +3134,13 @@
         <v>2</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
@@ -3295,13 +3295,13 @@
         <v>2</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
@@ -3456,13 +3456,13 @@
         <v>2</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
@@ -3617,13 +3617,13 @@
         <v>2</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
@@ -3778,13 +3778,13 @@
         <v>2</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
@@ -3802,13 +3802,13 @@
         <v>2</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
@@ -3963,13 +3963,13 @@
         <v>2</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
@@ -3987,13 +3987,13 @@
         <v>2</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
@@ -4011,13 +4011,13 @@
         <v>2</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
@@ -4035,13 +4035,13 @@
         <v>2</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
@@ -4059,13 +4059,13 @@
         <v>2</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
@@ -4083,13 +4083,13 @@
         <v>2</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
@@ -4107,13 +4107,13 @@
         <v>2</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
@@ -4131,13 +4131,13 @@
         <v>1</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
@@ -4155,13 +4155,13 @@
         <v>1</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
@@ -4179,13 +4179,13 @@
         <v>2</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>174</v>
+        <v>378</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
@@ -4203,13 +4203,13 @@
         <v>2</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
@@ -4227,13 +4227,13 @@
         <v>2</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
@@ -4388,13 +4388,13 @@
         <v>2</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
@@ -4549,13 +4549,13 @@
         <v>2</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
@@ -4710,13 +4710,13 @@
         <v>2</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
@@ -4734,13 +4734,13 @@
         <v>2</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
@@ -4758,13 +4758,13 @@
         <v>2</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
@@ -4782,13 +4782,13 @@
         <v>2</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
@@ -4943,13 +4943,13 @@
         <v>2</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
@@ -5104,13 +5104,13 @@
         <v>2</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
@@ -5128,13 +5128,13 @@
         <v>2</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
@@ -5152,13 +5152,13 @@
         <v>2</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
@@ -5176,13 +5176,13 @@
         <v>2</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
@@ -5200,13 +5200,13 @@
         <v>2</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
@@ -5224,13 +5224,13 @@
         <v>2</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
@@ -5248,13 +5248,13 @@
         <v>2</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
@@ -5272,13 +5272,13 @@
         <v>2</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
@@ -5296,13 +5296,13 @@
         <v>1</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>180</v>
+        <v>379</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
@@ -5320,13 +5320,13 @@
         <v>2</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D67" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
@@ -5481,13 +5481,13 @@
         <v>2</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
@@ -5642,13 +5642,13 @@
         <v>2</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
@@ -5666,13 +5666,13 @@
         <v>2</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
@@ -5690,13 +5690,13 @@
         <v>2</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
@@ -5714,13 +5714,13 @@
         <v>2</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
@@ -5738,13 +5738,13 @@
         <v>2</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
@@ -5762,13 +5762,13 @@
         <v>2</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
@@ -5786,13 +5786,13 @@
         <v>2</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
@@ -5810,13 +5810,13 @@
         <v>2</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
@@ -5834,13 +5834,13 @@
         <v>1</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>181</v>
+        <v>380</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
@@ -5858,13 +5858,13 @@
         <v>1</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
@@ -5882,13 +5882,13 @@
         <v>1</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
@@ -5906,13 +5906,13 @@
         <v>1</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
@@ -5930,13 +5930,13 @@
         <v>2</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
@@ -5954,13 +5954,13 @@
         <v>2</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
@@ -5978,13 +5978,13 @@
         <v>2</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
@@ -6002,13 +6002,13 @@
         <v>2</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
@@ -6163,13 +6163,13 @@
         <v>2</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
@@ -6317,20 +6317,20 @@
     </row>
     <row r="86" spans="1:145" s="14" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B86" s="12" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
@@ -6478,20 +6478,20 @@
     </row>
     <row r="87" spans="1:145" s="14" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B87" s="12" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
@@ -6639,20 +6639,20 @@
     </row>
     <row r="88" spans="1:145" s="14" customFormat="1" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B88" s="12" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
@@ -6800,20 +6800,20 @@
     </row>
     <row r="89" spans="1:145" s="15" customFormat="1" ht="56.6" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B89" s="12" t="str">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
@@ -6959,7 +6959,7 @@
       <c r="EN89" s="4"/>
       <c r="EO89" s="4"/>
     </row>
-    <row r="90" spans="1:145" ht="42.45" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:145" ht="56.6" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>17</v>
       </c>
@@ -6968,13 +6968,13 @@
         <v>1</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>182</v>
+        <v>381</v>
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
@@ -6992,13 +6992,13 @@
         <v>1</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
@@ -7016,13 +7016,13 @@
         <v>2</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
@@ -7040,13 +7040,13 @@
         <v>2</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
@@ -7064,13 +7064,13 @@
         <v>2</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
@@ -7088,13 +7088,13 @@
         <v>2</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
@@ -7112,13 +7112,13 @@
         <v>2</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
@@ -7136,13 +7136,13 @@
         <v>2</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
@@ -7160,13 +7160,13 @@
         <v>2</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
@@ -7184,13 +7184,13 @@
         <v>2</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F99" s="9"/>
       <c r="G99" s="8"/>
@@ -7208,13 +7208,13 @@
         <v>2</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
@@ -7232,13 +7232,13 @@
         <v>2</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
@@ -7256,13 +7256,13 @@
         <v>2</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
@@ -7280,13 +7280,13 @@
         <v>2</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
@@ -7304,13 +7304,13 @@
         <v>2</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
@@ -7328,10 +7328,10 @@
         <v>2</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E105" s="6" t="s">
         <v>18</v>
@@ -7352,13 +7352,13 @@
         <v>1</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
@@ -7376,13 +7376,13 @@
         <v>1</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
@@ -7400,13 +7400,13 @@
         <v>1</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
@@ -7424,13 +7424,13 @@
         <v>1</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
@@ -7448,13 +7448,13 @@
         <v>2</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="D110" s="14" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
@@ -7472,13 +7472,13 @@
         <v>2</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
@@ -7633,13 +7633,13 @@
         <v>2</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
@@ -7670,10 +7670,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D02293755B0C1C458CEABDE3487C809F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c73c4644de115ba955e1f8120af59752">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e084eb51-e41f-419d-868e-d827d41fdf42" xmlns:ns3="a54a5347-8adb-4f47-b158-08c1baf179b6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2083b23bc962d12d85d394e2a396312c" ns2:_="" ns3:_="">
-    <xsd:import namespace="e084eb51-e41f-419d-868e-d827d41fdf42"/>
-    <xsd:import namespace="a54a5347-8adb-4f47-b158-08c1baf179b6"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004082676A57B6E94690E98757219CADCB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f0cf3e001cba8a7a59f6ca10dce6da2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fb85b12d-9ea0-4af7-b89e-54842e89140c" xmlns:ns3="9e79c3b1-452c-4fb6-ac46-d68c59ca6476" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3f43e50843cd2526071d0b839d8f426" ns2:_="" ns3:_="">
+    <xsd:import namespace="fb85b12d-9ea0-4af7-b89e-54842e89140c"/>
+    <xsd:import namespace="9e79c3b1-452c-4fb6-ac46-d68c59ca6476"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -7682,15 +7682,17 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -7698,7 +7700,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e084eb51-e41f-419d-868e-d827d41fdf42" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fb85b12d-9ea0-4af7-b89e-54842e89140c" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -7711,50 +7713,60 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="15" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a54a5347-8adb-4f47-b158-08c1baf179b6" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9e79c3b1-452c-4fb6-ac46-d68c59ca6476" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -7773,7 +7785,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -7892,7 +7904,7 @@
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <SharedWithUsers xmlns="a54a5347-8adb-4f47-b158-08c1baf179b6">
+    <SharedWithUsers xmlns="9e79c3b1-452c-4fb6-ac46-d68c59ca6476">
       <UserInfo>
         <DisplayName>Kelly Hood</DisplayName>
         <AccountId>6</AccountId>
@@ -7909,22 +7921,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4239EBBD-2243-4F26-A9B0-A3B8F086CFF9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e084eb51-e41f-419d-868e-d827d41fdf42"/>
-    <ds:schemaRef ds:uri="a54a5347-8adb-4f47-b158-08c1baf179b6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88510C2C-AAE1-4D27-8EB5-E559F800F247}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>